<commit_message>
updated cheatsheet for test
</commit_message>
<xml_diff>
--- a/DB Phase 3/Seperate Excel Sheet Phase 3/Job_History.xlsx
+++ b/DB Phase 3/Seperate Excel Sheet Phase 3/Job_History.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C4056-DEBE-4B74-834C-7A6BBB5651F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E77684-BF1A-477C-8B86-B9EAF9CCACE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24405" yWindow="4485" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,9 +413,10 @@
     <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -445,8 +446,9 @@
       <c r="D2" s="1">
         <v>42050</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -462,8 +464,9 @@
       <c r="E3" s="1">
         <v>42520</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -479,8 +482,9 @@
       <c r="E4" s="1">
         <v>42437</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -496,8 +500,9 @@
       <c r="E5" s="1">
         <v>41746</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -510,8 +515,9 @@
       <c r="D6" s="1">
         <v>41706</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -528,7 +534,7 @@
         <v>42024</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -542,7 +548,7 @@
         <v>42778</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -556,7 +562,7 @@
         <v>41653</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -570,7 +576,7 @@
         <v>41997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -584,7 +590,7 @@
         <v>41855</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -598,7 +604,7 @@
         <v>42042</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -612,7 +618,7 @@
         <v>42521</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>